<commit_message>
Created a summary table of proportions
</commit_message>
<xml_diff>
--- a/proportion_calculations.xlsx
+++ b/proportion_calculations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="42">
   <si>
     <t>&lt;1 sq m</t>
   </si>
@@ -115,6 +115,36 @@
   </si>
   <si>
     <t>Proportion of studies that took a single sample after the event</t>
+  </si>
+  <si>
+    <t>Study Spatial Extent</t>
+  </si>
+  <si>
+    <t>Sampling Unit Spatial Extent</t>
+  </si>
+  <si>
+    <t>Sampling Duration Before</t>
+  </si>
+  <si>
+    <t>Sampling Duration During</t>
+  </si>
+  <si>
+    <t>Sampling Duration After</t>
+  </si>
+  <si>
+    <t>Proportion of studies that sample on the same scale as the event</t>
+  </si>
+  <si>
+    <t>Proportion of studies that didn't sample</t>
+  </si>
+  <si>
+    <t>Proportion of studies that didn't sample after the event</t>
+  </si>
+  <si>
+    <t>Proportion of studies that took a single sample</t>
+  </si>
+  <si>
+    <t>--</t>
   </si>
 </sst>
 </file>
@@ -127,6 +157,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -154,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -242,8 +273,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -267,14 +335,57 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -285,14 +396,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="69">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -304,6 +452,29 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -315,6 +486,29 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -644,44 +838,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="3"/>
-      <c r="C2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="J2" t="s">
@@ -689,25 +885,25 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
         <v>5.2910052910052898E-3</v>
       </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6">
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
         <v>0</v>
       </c>
       <c r="J3">
@@ -716,159 +912,159 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="2"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5">
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
         <v>0.46560846560846603</v>
       </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6">
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
         <v>0.13227513227513199</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="2"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="13"/>
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>5.2910052910052898E-3</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>1.58730158730159E-2</v>
       </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
         <v>3.7037037037037E-2</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="13"/>
+      <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
         <v>2.6455026455026499E-2</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>8.99470899470899E-2</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>1.0582010582010601E-2</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="2"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="13"/>
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
         <v>3.1746031746031703E-2</v>
       </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0</v>
-      </c>
-      <c r="G7" s="6">
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
         <v>5.2910052910052898E-3</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="2"/>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5">
-        <v>0</v>
-      </c>
-      <c r="D8" s="5">
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
         <v>5.2910052910052898E-3</v>
       </c>
-      <c r="E8" s="5">
-        <v>0</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0</v>
-      </c>
-      <c r="G8" s="6">
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
         <v>0.13227513227513199</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="2"/>
-      <c r="B9" s="11" t="s">
+      <c r="A9" s="13"/>
+      <c r="B9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="7">
-        <v>0</v>
-      </c>
-      <c r="D9" s="7">
-        <v>0</v>
-      </c>
-      <c r="E9" s="7">
-        <v>0</v>
-      </c>
-      <c r="F9" s="7">
-        <v>0</v>
-      </c>
-      <c r="G9" s="8">
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="7">
         <v>3.7037037037037E-2</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="9" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="9" t="s">
         <v>4</v>
       </c>
       <c r="J12" t="s">
@@ -876,23 +1072,23 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="2"/>
-      <c r="B13" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="5">
+      <c r="A13" s="13"/>
+      <c r="B13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4">
         <v>5.2910052910052898E-3</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>0.16402116402116401</v>
       </c>
-      <c r="E13" s="5">
-        <v>0</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0</v>
-      </c>
-      <c r="G13" s="6">
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
         <v>0.11640211640211599</v>
       </c>
       <c r="J13">
@@ -901,128 +1097,128 @@
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="2"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="13"/>
+      <c r="B14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="5">
-        <v>0</v>
-      </c>
-      <c r="D14" s="5">
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
         <v>8.4656084656084707E-2</v>
       </c>
-      <c r="E14" s="5">
-        <v>0</v>
-      </c>
-      <c r="F14" s="5">
-        <v>0</v>
-      </c>
-      <c r="G14" s="6">
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
         <v>2.1164021164021201E-2</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="2"/>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="13"/>
+      <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="5">
-        <v>0</v>
-      </c>
-      <c r="D15" s="5">
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
         <v>3.1746031746031703E-2</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>6.8783068783068793E-2</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>1.0582010582010601E-2</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <v>0.12169312169312201</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="2"/>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="13"/>
+      <c r="B16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="5">
-        <v>0</v>
-      </c>
-      <c r="D16" s="5">
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
         <v>4.7619047619047603E-2</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>2.1164021164021201E-2</v>
       </c>
-      <c r="F16" s="5">
-        <v>0</v>
-      </c>
-      <c r="G16" s="6">
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="5">
         <v>1.58730158730159E-2</v>
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="2"/>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="13"/>
+      <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="5">
-        <v>0</v>
-      </c>
-      <c r="D17" s="5">
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
         <v>0.13227513227513199</v>
       </c>
-      <c r="E17" s="5">
-        <v>0</v>
-      </c>
-      <c r="F17" s="5">
-        <v>0</v>
-      </c>
-      <c r="G17" s="6">
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5">
         <v>5.2910052910052898E-3</v>
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="2"/>
-      <c r="B18" s="4" t="s">
+      <c r="A18" s="13"/>
+      <c r="B18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="5">
-        <v>0</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0</v>
-      </c>
-      <c r="E18" s="5">
-        <v>0</v>
-      </c>
-      <c r="F18" s="5">
-        <v>0</v>
-      </c>
-      <c r="G18" s="6">
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5">
         <v>2.6455026455026499E-2</v>
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="2"/>
-      <c r="B19" s="11" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="7">
-        <v>0</v>
-      </c>
-      <c r="D19" s="7">
+      <c r="C19" s="6">
+        <v>0</v>
+      </c>
+      <c r="D19" s="6">
         <v>8.99470899470899E-2</v>
       </c>
-      <c r="E19" s="7">
-        <v>0</v>
-      </c>
-      <c r="F19" s="7">
-        <v>0</v>
-      </c>
-      <c r="G19" s="8">
+      <c r="E19" s="6">
+        <v>0</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0</v>
+      </c>
+      <c r="G19" s="7">
         <v>3.7037037037037E-2</v>
       </c>
     </row>
@@ -1040,23 +1236,23 @@
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="9" t="s">
+      <c r="B22" s="2"/>
+      <c r="C22" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="9" t="s">
         <v>17</v>
       </c>
       <c r="J22">
@@ -1065,44 +1261,44 @@
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="13"/>
-      <c r="B23" s="4" t="s">
+      <c r="A23" s="11"/>
+      <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>1.5228426395939101E-2</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="4">
         <v>3.0456852791878201E-2</v>
       </c>
-      <c r="E23" s="5">
-        <v>0</v>
-      </c>
-      <c r="F23" s="5">
-        <v>0</v>
-      </c>
-      <c r="G23" s="6">
+      <c r="E23" s="4">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="13"/>
-      <c r="B24" s="4" t="s">
+      <c r="A24" s="11"/>
+      <c r="B24" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <v>2.5380710659898501E-2</v>
       </c>
-      <c r="D24" s="5">
-        <v>0</v>
-      </c>
-      <c r="E24" s="5">
+      <c r="D24" s="4">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4">
         <v>0.131979695431472</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="4">
         <v>4.5685279187817299E-2</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="5">
         <v>0</v>
       </c>
       <c r="J24" t="s">
@@ -1110,23 +1306,23 @@
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="13"/>
-      <c r="B25" s="4" t="s">
+      <c r="A25" s="11"/>
+      <c r="B25" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <v>5.0761421319797002E-3</v>
       </c>
-      <c r="D25" s="5">
-        <v>0</v>
-      </c>
-      <c r="E25" s="5">
+      <c r="D25" s="4">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4">
         <v>0.14213197969543101</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="4">
         <v>1.5228426395939101E-2</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="5">
         <v>0.101522842639594</v>
       </c>
       <c r="J25">
@@ -1135,44 +1331,44 @@
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="13"/>
-      <c r="B26" s="4" t="s">
+      <c r="A26" s="11"/>
+      <c r="B26" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="5">
-        <v>0</v>
-      </c>
-      <c r="D26" s="5">
-        <v>0</v>
-      </c>
-      <c r="E26" s="5">
+      <c r="C26" s="4">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4">
         <v>5.0761421319797002E-3</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="4">
         <v>1.5228426395939101E-2</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="13"/>
-      <c r="B27" s="4" t="s">
+      <c r="A27" s="11"/>
+      <c r="B27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="5">
-        <v>0</v>
-      </c>
-      <c r="D27" s="5">
-        <v>0</v>
-      </c>
-      <c r="E27" s="5">
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4">
         <v>5.0761421319797002E-3</v>
       </c>
-      <c r="F27" s="5">
-        <v>0</v>
-      </c>
-      <c r="G27" s="6">
+      <c r="F27" s="4">
+        <v>0</v>
+      </c>
+      <c r="G27" s="5">
         <v>0</v>
       </c>
       <c r="J27" t="s">
@@ -1180,23 +1376,23 @@
       </c>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="13"/>
-      <c r="B28" s="11" t="s">
+      <c r="A28" s="11"/>
+      <c r="B28" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="6">
         <v>7.6142131979695396E-2</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="6">
         <v>5.0761421319797002E-2</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="6">
         <v>0.19796954314720799</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="6">
         <v>2.0304568527918801E-2</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G28" s="7">
         <v>0.116751269035533</v>
       </c>
       <c r="J28">
@@ -1215,20 +1411,20 @@
       <c r="G30" s="12"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="B31" s="3"/>
-      <c r="C31" s="9" t="s">
+      <c r="B31" s="2"/>
+      <c r="C31" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="F31" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G31" s="9" t="s">
         <v>17</v>
       </c>
       <c r="J31" t="s">
@@ -1236,25 +1432,25 @@
       </c>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="4">
         <v>1.5228426395939101E-2</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="4">
         <v>5.0761421319797002E-2</v>
       </c>
-      <c r="E32" s="5">
-        <v>0</v>
-      </c>
-      <c r="F32" s="5">
-        <v>0</v>
-      </c>
-      <c r="G32" s="6">
+      <c r="E32" s="4">
+        <v>0</v>
+      </c>
+      <c r="F32" s="4">
+        <v>0</v>
+      </c>
+      <c r="G32" s="5">
         <v>0</v>
       </c>
       <c r="J32">
@@ -1263,44 +1459,44 @@
       </c>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="13"/>
-      <c r="B33" s="4" t="s">
+      <c r="A33" s="11"/>
+      <c r="B33" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="4">
         <v>5.0761421319797002E-3</v>
       </c>
-      <c r="D33" s="5">
-        <v>0</v>
-      </c>
-      <c r="E33" s="5">
+      <c r="D33" s="4">
+        <v>0</v>
+      </c>
+      <c r="E33" s="4">
         <v>3.0456852791878201E-2</v>
       </c>
-      <c r="F33" s="5">
-        <v>0</v>
-      </c>
-      <c r="G33" s="6">
+      <c r="F33" s="4">
+        <v>0</v>
+      </c>
+      <c r="G33" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="13"/>
-      <c r="B34" s="4" t="s">
+      <c r="A34" s="11"/>
+      <c r="B34" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="4">
         <v>5.0761421319797002E-3</v>
       </c>
-      <c r="D34" s="5">
-        <v>0</v>
-      </c>
-      <c r="E34" s="5">
+      <c r="D34" s="4">
+        <v>0</v>
+      </c>
+      <c r="E34" s="4">
         <v>0.26395939086294401</v>
       </c>
-      <c r="F34" s="5">
+      <c r="F34" s="4">
         <v>4.0609137055837602E-2</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G34" s="5">
         <v>3.5532994923857898E-2</v>
       </c>
       <c r="J34" t="s">
@@ -1308,23 +1504,23 @@
       </c>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="13"/>
-      <c r="B35" s="4" t="s">
+      <c r="A35" s="11"/>
+      <c r="B35" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="4">
         <v>3.5532994923857898E-2</v>
       </c>
-      <c r="D35" s="5">
-        <v>0</v>
-      </c>
-      <c r="E35" s="5">
+      <c r="D35" s="4">
+        <v>0</v>
+      </c>
+      <c r="E35" s="4">
         <v>0.14213197969543101</v>
       </c>
-      <c r="F35" s="5">
+      <c r="F35" s="4">
         <v>1.5228426395939101E-2</v>
       </c>
-      <c r="G35" s="6">
+      <c r="G35" s="5">
         <v>5.0761421319797002E-3</v>
       </c>
       <c r="J35">
@@ -1333,44 +1529,44 @@
       </c>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="13"/>
-      <c r="B36" s="4" t="s">
+      <c r="A36" s="11"/>
+      <c r="B36" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="5">
-        <v>0</v>
-      </c>
-      <c r="D36" s="5">
+      <c r="C36" s="4">
+        <v>0</v>
+      </c>
+      <c r="D36" s="4">
         <v>3.0456852791878201E-2</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="4">
         <v>2.0304568527918801E-2</v>
       </c>
-      <c r="F36" s="5">
+      <c r="F36" s="4">
         <v>1.5228426395939101E-2</v>
       </c>
-      <c r="G36" s="6">
+      <c r="G36" s="5">
         <v>8.1218274111675107E-2</v>
       </c>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="13"/>
-      <c r="B37" s="4" t="s">
+      <c r="A37" s="11"/>
+      <c r="B37" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="5">
-        <v>0</v>
-      </c>
-      <c r="D37" s="5">
-        <v>0</v>
-      </c>
-      <c r="E37" s="5">
+      <c r="C37" s="4">
+        <v>0</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0</v>
+      </c>
+      <c r="E37" s="4">
         <v>5.0761421319797002E-3</v>
       </c>
-      <c r="F37" s="5">
+      <c r="F37" s="4">
         <v>1.01522842639594E-2</v>
       </c>
-      <c r="G37" s="6">
+      <c r="G37" s="5">
         <v>0</v>
       </c>
       <c r="J37" t="s">
@@ -1378,23 +1574,23 @@
       </c>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="13"/>
-      <c r="B38" s="11" t="s">
+      <c r="A38" s="11"/>
+      <c r="B38" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="6">
         <v>6.0913705583756299E-2</v>
       </c>
-      <c r="D38" s="7">
-        <v>0</v>
-      </c>
-      <c r="E38" s="7">
+      <c r="D38" s="6">
+        <v>0</v>
+      </c>
+      <c r="E38" s="6">
         <v>2.0304568527918801E-2</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="6">
         <v>1.5228426395939101E-2</v>
       </c>
-      <c r="G38" s="8">
+      <c r="G38" s="7">
         <v>9.6446700507614197E-2</v>
       </c>
       <c r="J38">
@@ -1413,20 +1609,20 @@
       <c r="G40" s="12"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="B41" s="3"/>
-      <c r="C41" s="9" t="s">
+      <c r="B41" s="2"/>
+      <c r="C41" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D41" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="E41" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F41" s="9" t="s">
+      <c r="F41" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G41" s="10" t="s">
+      <c r="G41" s="9" t="s">
         <v>17</v>
       </c>
       <c r="J41" t="s">
@@ -1434,25 +1630,25 @@
       </c>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="4">
         <v>1.5228426395939101E-2</v>
       </c>
-      <c r="D42" s="5">
-        <v>0</v>
-      </c>
-      <c r="E42" s="5">
-        <v>0</v>
-      </c>
-      <c r="F42" s="5">
-        <v>0</v>
-      </c>
-      <c r="G42" s="6">
+      <c r="D42" s="4">
+        <v>0</v>
+      </c>
+      <c r="E42" s="4">
+        <v>0</v>
+      </c>
+      <c r="F42" s="4">
+        <v>0</v>
+      </c>
+      <c r="G42" s="5">
         <v>0</v>
       </c>
       <c r="J42">
@@ -1461,68 +1657,68 @@
       </c>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="13"/>
-      <c r="B43" s="4" t="s">
+      <c r="A43" s="11"/>
+      <c r="B43" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="4">
         <v>1.01522842639594E-2</v>
       </c>
-      <c r="D43" s="5">
-        <v>0</v>
-      </c>
-      <c r="E43" s="5">
+      <c r="D43" s="4">
+        <v>0</v>
+      </c>
+      <c r="E43" s="4">
         <v>0.21319796954314699</v>
       </c>
-      <c r="F43" s="5">
+      <c r="F43" s="4">
         <v>4.5685279187817299E-2</v>
       </c>
-      <c r="G43" s="6">
+      <c r="G43" s="5">
         <v>3.5532994923857898E-2</v>
       </c>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="13"/>
-      <c r="B44" s="4" t="s">
+      <c r="A44" s="11"/>
+      <c r="B44" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="4">
         <v>5.5837563451776699E-2</v>
       </c>
-      <c r="D44" s="5">
-        <v>0</v>
-      </c>
-      <c r="E44" s="5">
+      <c r="D44" s="4">
+        <v>0</v>
+      </c>
+      <c r="E44" s="4">
         <v>5.5837563451776699E-2</v>
       </c>
-      <c r="F44" s="5">
+      <c r="F44" s="4">
         <v>5.0761421319797002E-3</v>
       </c>
-      <c r="G44" s="6">
+      <c r="G44" s="5">
         <v>6.5989847715736002E-2</v>
       </c>
       <c r="J44" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="13"/>
-      <c r="B45" s="4" t="s">
+      <c r="A45" s="11"/>
+      <c r="B45" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C45" s="5">
-        <v>0</v>
-      </c>
-      <c r="D45" s="5">
-        <v>0</v>
-      </c>
-      <c r="E45" s="5">
+      <c r="C45" s="4">
+        <v>0</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0</v>
+      </c>
+      <c r="E45" s="4">
         <v>1.5228426395939101E-2</v>
       </c>
-      <c r="F45" s="5">
+      <c r="F45" s="4">
         <v>3.0456852791878201E-2</v>
       </c>
-      <c r="G45" s="6">
+      <c r="G45" s="5">
         <v>0</v>
       </c>
       <c r="J45">
@@ -1531,44 +1727,44 @@
       </c>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="13"/>
-      <c r="B46" s="4" t="s">
+      <c r="A46" s="11"/>
+      <c r="B46" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C46" s="5">
-        <v>0</v>
-      </c>
-      <c r="D46" s="5">
+      <c r="C46" s="4">
+        <v>0</v>
+      </c>
+      <c r="D46" s="4">
         <v>3.0456852791878201E-2</v>
       </c>
-      <c r="E46" s="5">
+      <c r="E46" s="4">
         <v>1.01522842639594E-2</v>
       </c>
-      <c r="F46" s="5">
-        <v>0</v>
-      </c>
-      <c r="G46" s="6">
+      <c r="F46" s="4">
+        <v>0</v>
+      </c>
+      <c r="G46" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="13"/>
-      <c r="B47" s="11" t="s">
+      <c r="A47" s="11"/>
+      <c r="B47" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C47" s="6">
         <v>4.0609137055837602E-2</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="6">
         <v>5.0761421319797002E-2</v>
       </c>
-      <c r="E47" s="7">
+      <c r="E47" s="6">
         <v>0.18781725888324899</v>
       </c>
-      <c r="F47" s="7">
+      <c r="F47" s="6">
         <v>1.5228426395939101E-2</v>
       </c>
-      <c r="G47" s="8">
+      <c r="G47" s="7">
         <v>0.116751269035533</v>
       </c>
       <c r="J47" t="s">
@@ -1576,24 +1772,109 @@
       </c>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="13"/>
+      <c r="A48" s="11"/>
       <c r="J48">
         <f>C45+D45+E45+F45+G45</f>
         <v>4.5685279187817299E-2</v>
       </c>
     </row>
+    <row r="50" spans="1:5" ht="60">
+      <c r="A50" s="1"/>
+      <c r="B50" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E50" s="16"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" s="21">
+        <v>0.6878306878306879</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E51" s="15"/>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B52" s="23">
+        <v>0.1375661375661377</v>
+      </c>
+      <c r="C52" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D52" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E52" s="15"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B53" s="23">
+        <v>0.26395939086294412</v>
+      </c>
+      <c r="C53" s="23">
+        <v>0.26395939086294384</v>
+      </c>
+      <c r="D53" s="23">
+        <v>2.0304568527918801E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="23">
+        <v>0.38578680203045668</v>
+      </c>
+      <c r="C54" s="23">
+        <v>0.19796954314720772</v>
+      </c>
+      <c r="D54" s="23">
+        <v>0.14720812182741122</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" s="25">
+        <v>0.3451776649746191</v>
+      </c>
+      <c r="C55" s="25">
+        <v>0.18274111675126908</v>
+      </c>
+      <c r="D55" s="25">
+        <v>4.5685279187817299E-2</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="A12:A19"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="A22:A28"/>
     <mergeCell ref="A32:A38"/>
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="A42:A48"/>
     <mergeCell ref="B40:G40"/>
     <mergeCell ref="A3:A9"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="A12:A19"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="A22:A28"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
change data import code, unique analysis
</commit_message>
<xml_diff>
--- a/proportion_calculations.xlsx
+++ b/proportion_calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="0" windowWidth="25040" windowHeight="14000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25040" windowHeight="22000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="proportion_calculations.csv" sheetId="1" r:id="rId1"/>
@@ -132,19 +132,19 @@
     <t>Sampling Duration After</t>
   </si>
   <si>
-    <t>Proportion of studies that sample on the same scale as the event</t>
-  </si>
-  <si>
-    <t>Proportion of studies that didn't sample</t>
-  </si>
-  <si>
     <t>Proportion of studies that didn't sample after the event</t>
   </si>
   <si>
-    <t>Proportion of studies that took a single sample</t>
-  </si>
-  <si>
     <t>--</t>
+  </si>
+  <si>
+    <t>a) Proportion of studies that sample on the same scale as the event</t>
+  </si>
+  <si>
+    <t>b) Proportion of studies that didn't sample</t>
+  </si>
+  <si>
+    <t>c) Proportion of studies that took a single sample</t>
   </si>
 </sst>
 </file>
@@ -311,8 +311,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -440,7 +462,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="91">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -475,6 +497,17 @@
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -509,6 +542,17 @@
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -840,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:D55"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1698,7 +1742,7 @@
         <v>6.5989847715736002E-2</v>
       </c>
       <c r="J44" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -1781,13 +1825,13 @@
     <row r="50" spans="1:5" ht="60">
       <c r="A50" s="1"/>
       <c r="B50" s="17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E50" s="16"/>
     </row>
@@ -1799,10 +1843,10 @@
         <v>0.6878306878306879</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E51" s="15"/>
     </row>
@@ -1814,10 +1858,10 @@
         <v>0.1375661375661377</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E52" s="15"/>
     </row>

</xml_diff>